<commit_message>
Fixed error in code causing growth to look like N
</commit_message>
<xml_diff>
--- a/M2/Programming Assignment/TreeInsertData.xlsx
+++ b/M2/Programming Assignment/TreeInsertData.xlsx
@@ -8,15 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colin\Documents\GitHub\AlgorithmsII_Assignments\M2\Programming Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDE597BD-F839-4D75-8F7A-9107581A393A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D2D9A90E-C605-43D5-800D-E28D2A50892E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="1425" windowWidth="16440" windowHeight="28440"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>average height</t>
+  </si>
+  <si>
+    <t>height / n</t>
+  </si>
+  <si>
+    <t>height / log n</t>
+  </si>
+  <si>
+    <t>log 2 n</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -556,6 +576,1039 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>height / log n</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data!$D$2:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>2.1191676485573727</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2075533015358619</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2747204997137298</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1886259456671016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1262058416266951</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2509367128453888</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2084169348103964</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1728621694548824</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3896419497462342</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.360081283173991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.3339634679747783</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.3106194791351986</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.2895536975804291</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.3486787010210932</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.330517959867044</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.3137821315975917</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.3748880030364923</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.4361075068744991</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.3460478383102155</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.3329824663958543</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.3206890229569153</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.3835743298650169</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.3722424666811817</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.4352901373373785</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.3512744557878711</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.3415392571815192</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.3322473197504849</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.3959679419997317</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.3148541191439347</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.3066928531216178</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.2988537793926027</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.3629177801523276</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.4268070697974071</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.348211748098568</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.4121913909643746</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.2637703812610552</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.2574577435280601</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.3217017812615324</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.3155966692204233</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.3796671641196743</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D13E-4A27-8BF1-B722CE7A86A3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1764364495"/>
+        <c:axId val="1417944719"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1764364495"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1417944719"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1417944719"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1764364495"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>504824</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>74612</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>311149</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E8E3026-ED39-4E30-8BC4-BBCDC6A0FDDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -855,333 +1908,837 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="3" max="4" width="12.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>500</v>
       </c>
-      <c r="B1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="B2">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <f>(B2/A2)</f>
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D2">
+        <f>(B2/G2)</f>
+        <v>2.1191676485573727</v>
+      </c>
+      <c r="G2">
+        <f>LOG(A2, 2)</f>
+        <v>8.965784284662087</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>1000</v>
       </c>
-      <c r="B2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C41" si="0">(B3/A3)</f>
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D41" si="1">(B3/G3)</f>
+        <v>2.2075533015358619</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G41" si="2">LOG(A3, 2)</f>
+        <v>9.965784284662087</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>1500</v>
       </c>
-      <c r="B3">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="B4">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>1.6E-2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>2.2747204997137298</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>10.550746785383243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>2000</v>
       </c>
-      <c r="B4">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="B5">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>1.2E-2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>2.1886259456671016</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>10.965784284662087</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>2500</v>
       </c>
-      <c r="B5">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="B6">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>2.1262058416266951</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>11.287712379549449</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>3000</v>
       </c>
-      <c r="B6">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="B7">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>8.6666666666666663E-3</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>2.2509367128453888</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>11.550746785383243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8">
         <v>3500</v>
       </c>
-      <c r="B7">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="B8">
+        <v>26</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>7.4285714285714285E-3</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>2.2084169348103964</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>11.773139206719691</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9">
         <v>4000</v>
       </c>
-      <c r="B8">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="B9">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>2.1728621694548824</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>11.965784284662087</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10">
         <v>4500</v>
       </c>
-      <c r="B9">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="B10">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>6.4444444444444445E-3</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>2.3896419497462342</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>12.135709286104401</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11">
         <v>5000</v>
       </c>
-      <c r="B10">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="B11">
+        <v>29</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>2.360081283173991</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>12.287712379549451</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12">
         <v>5500</v>
       </c>
-      <c r="B11">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="B12">
+        <v>29</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>5.2727272727272727E-3</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>2.3339634679747783</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>12.425215903299385</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13">
         <v>6000</v>
       </c>
-      <c r="B12">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="B13">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>4.8333333333333336E-3</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>2.3106194791351986</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>12.550746785383243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14">
         <v>6500</v>
       </c>
-      <c r="B13">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="B14">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>4.4615384615384612E-3</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>2.2895536975804291</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>12.666224002803178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15">
         <v>7000</v>
       </c>
-      <c r="B14">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="B15">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>4.2857142857142859E-3</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>2.3486787010210932</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>12.773139206719691</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16">
         <v>7500</v>
       </c>
-      <c r="B15">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16">
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>2.330517959867044</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>12.872674880270607</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17">
         <v>8000</v>
       </c>
-      <c r="B16">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17">
+      <c r="B17">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>3.7499999999999999E-3</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>2.3137821315975917</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>12.965784284662087</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18">
         <v>8500</v>
       </c>
-      <c r="B17">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18">
+      <c r="B18">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>3.6470588235294117E-3</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>2.3748880030364923</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>13.053247125912428</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19">
         <v>9000</v>
       </c>
-      <c r="B18">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="B19">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>3.5555555555555557E-3</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>2.4361075068744991</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>13.135709286104401</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20">
         <v>9500</v>
       </c>
-      <c r="B19">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20">
+      <c r="B20">
+        <v>31</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>3.2631578947368419E-3</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>2.3460478383102155</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>13.213711798105672</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21">
         <v>10000</v>
       </c>
-      <c r="B20">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21">
+      <c r="B21">
+        <v>31</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>3.0999999999999999E-3</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>2.3329824663958543</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>13.287712379549451</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22">
         <v>10500</v>
       </c>
-      <c r="B21">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22">
+      <c r="B22">
+        <v>31</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>2.9523809523809524E-3</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>2.3206890229569153</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>13.358101707440847</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23">
         <v>11000</v>
       </c>
-      <c r="B22">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23">
+      <c r="B23">
+        <v>32</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>2.9090909090909089E-3</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>2.3835743298650169</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>13.425215903299385</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24">
         <v>11500</v>
       </c>
-      <c r="B23">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24">
+      <c r="B24">
+        <v>32</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>2.7826086956521741E-3</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>2.3722424666811817</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>13.489346240719099</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25">
         <v>12000</v>
       </c>
-      <c r="B24">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25">
+      <c r="B25">
+        <v>33</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>2.7499999999999998E-3</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>2.4352901373373785</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>13.550746785383243</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26">
         <v>12500</v>
       </c>
-      <c r="B25">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26">
+      <c r="B26">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>2.5600000000000002E-3</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>2.3512744557878711</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>13.609640474436812</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27">
         <v>13000</v>
       </c>
-      <c r="B26">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27">
+      <c r="B27">
+        <v>32</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>2.4615384615384616E-3</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>2.3415392571815192</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>13.666224002803178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28">
         <v>13500</v>
       </c>
-      <c r="B27">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28">
+      <c r="B28">
+        <v>32</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>2.3703703703703703E-3</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>2.3322473197504849</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="2"/>
+        <v>13.720671786825555</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29">
         <v>14000</v>
       </c>
-      <c r="B28">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29">
+      <c r="B29">
+        <v>33</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>2.3571428571428571E-3</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>2.3959679419997317</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="2"/>
+        <v>13.773139206719692</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30">
         <v>14500</v>
       </c>
-      <c r="B29">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30">
+      <c r="B30">
+        <v>32</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>2.206896551724138E-3</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>2.3148541191439347</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="2"/>
+        <v>13.82376527978966</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31">
         <v>15000</v>
       </c>
-      <c r="B30">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31">
+      <c r="B31">
+        <v>32</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>2.1333333333333334E-3</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>2.3066928531216178</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="2"/>
+        <v>13.872674880270607</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32">
         <v>15500</v>
       </c>
-      <c r="B31">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32">
+      <c r="B32">
+        <v>32</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>2.0645161290322581E-3</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>2.2988537793926027</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="2"/>
+        <v>13.919980595048964</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33">
         <v>16000</v>
       </c>
-      <c r="B32">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33">
+      <c r="B33">
+        <v>33</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>2.0625000000000001E-3</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>2.3629177801523276</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="2"/>
+        <v>13.965784284662087</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34">
         <v>16500</v>
       </c>
-      <c r="B33">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34">
+      <c r="B34">
+        <v>34</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>2.0606060606060605E-3</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>2.4268070697974071</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="2"/>
+        <v>14.010178404020539</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35">
         <v>17000</v>
       </c>
-      <c r="B34">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35">
+      <c r="B35">
+        <v>33</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>1.9411764705882352E-3</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>2.348211748098568</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="2"/>
+        <v>14.053247125912428</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36">
         <v>17500</v>
       </c>
-      <c r="B35">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36">
+      <c r="B36">
+        <v>34</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>1.9428571428571429E-3</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>2.4121913909643746</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="2"/>
+        <v>14.095067301607056</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37">
         <v>18000</v>
       </c>
-      <c r="B36">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37">
+      <c r="B37">
+        <v>32</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>1.7777777777777779E-3</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>2.2637703812610552</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="2"/>
+        <v>14.135709286104401</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38">
         <v>18500</v>
       </c>
-      <c r="B37">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38">
+      <c r="B38">
+        <v>32</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>1.7297297297297297E-3</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>2.2574577435280601</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="2"/>
+        <v>14.175237650291036</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39">
         <v>19000</v>
       </c>
-      <c r="B38">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39">
+      <c r="B39">
+        <v>33</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>1.7368421052631579E-3</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>2.3217017812615324</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="2"/>
+        <v>14.213711798105672</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40">
         <v>19500</v>
       </c>
-      <c r="B39">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40">
+      <c r="B40">
+        <v>33</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>1.6923076923076924E-3</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>2.3155966692204233</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="2"/>
+        <v>14.251186503524336</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41">
         <v>20000</v>
       </c>
-      <c r="B40">
-        <v>667</v>
+      <c r="B41">
+        <v>34</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>2.3796671641196743</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="2"/>
+        <v>14.287712379549449</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created word document - added graph to excel
</commit_message>
<xml_diff>
--- a/M2/Programming Assignment/TreeInsertData.xlsx
+++ b/M2/Programming Assignment/TreeInsertData.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colin\Documents\GitHub\AlgorithmsII_Assignments\M2\Programming Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D2D9A90E-C605-43D5-800D-E28D2A50892E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE3A1A4-49EC-408C-B08E-709564300B5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -40,7 +51,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1014,7 +1025,1456 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>height / n</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10500</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11500</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13500</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14500</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>16500</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17500</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>18500</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>19500</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$C$2:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.5999999999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6666666666666663E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.4285714285714285E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.4999999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.4444444444444445E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.7999999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.2727272727272727E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.8333333333333336E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.4615384615384612E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.2857142857142859E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.7499999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.6470588235294117E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.5555555555555557E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.2631578947368419E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.0999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.9523809523809524E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.9090909090909089E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.7826086956521741E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.7499999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.5600000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.4615384615384616E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.3703703703703703E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.3571428571428571E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.206896551724138E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.1333333333333334E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.0645161290322581E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.0625000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.0606060606060605E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.9411764705882352E-3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.9428571428571429E-3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.7777777777777779E-3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.7297297297297297E-3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.7368421052631579E-3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.6923076923076924E-3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.6999999999999999E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1A8D-4F4F-B681-1AC1358D1938}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="264982656"/>
+        <c:axId val="84406512"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="264982656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="84406512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="84406512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="264982656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>height vs log n</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Height</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$A$2:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10500</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11500</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13500</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14500</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>16500</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17500</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>18500</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>19500</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$B$2:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-01F5-4F20-9837-6F5DEF09F77C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>log n</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$A$2:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10500</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11500</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13500</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14500</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>16500</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17500</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>18500</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>19500</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$G$2:$G$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>8.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.550746785383243</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.287712379549449</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.550746785383243</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.773139206719691</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.135709286104401</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.287712379549451</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.425215903299385</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.550746785383243</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.666224002803178</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12.773139206719691</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12.872674880270607</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13.053247125912428</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13.135709286104401</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13.213711798105672</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13.287712379549451</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13.358101707440847</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13.425215903299385</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13.489346240719099</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>13.550746785383243</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>13.609640474436812</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13.666224002803178</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13.720671786825555</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13.773139206719692</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13.82376527978966</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>13.872674880270607</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>13.919980595048964</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>13.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>14.010178404020539</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>14.053247125912428</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>14.095067301607056</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>14.135709286104401</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>14.175237650291036</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>14.213711798105672</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>14.251186503524336</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>14.287712379549449</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-01F5-4F20-9837-6F5DEF09F77C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="359899872"/>
+        <c:axId val="278407248"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="359899872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="278407248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="278407248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="359899872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1570,20 +3030,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>504824</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>74612</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3174</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>311149</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>50799</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1603,6 +4095,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3174</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{326C4F7B-86FC-4597-9C3D-9F24CA43A70C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3174</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>60325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>44449</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{926FD52E-C04C-4C1F-9129-2F428ADCA8A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1907,11 +4471,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>